<commit_message>
ahp added almost working
</commit_message>
<xml_diff>
--- a/lol.xlsx
+++ b/lol.xlsx
@@ -2063,247 +2063,245 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>8.743415893791914</v>
+        <v>2.686192441575164</v>
       </c>
       <c r="C46" t="n">
-        <v>18485.6</v>
+        <v>4940.8</v>
       </c>
       <c r="D46" t="n">
-        <v>0.04002778947189373</v>
+        <v>0.01922476690873743</v>
       </c>
       <c r="E46" t="n">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="F46" t="n">
-        <v>229.6</v>
+        <v>215.4</v>
       </c>
       <c r="G46" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H46" t="s">
         <v>11</v>
       </c>
       <c r="I46" t="n">
-        <v>0.1242981404229443</v>
+        <v>0.1187514263010913</v>
       </c>
       <c r="J46" t="n">
-        <v>10</v>
+        <v>6.2</v>
       </c>
       <c r="K46" t="n">
-        <v>0.00490817992779415</v>
+        <v>0.003086678567510356</v>
       </c>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="1" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B47" t="n">
-        <v>2.686192441575164</v>
+        <v>3.753610964681075</v>
       </c>
       <c r="C47" t="n">
-        <v>4940.8</v>
+        <v>7120.6</v>
       </c>
       <c r="D47" t="n">
-        <v>0.01922476690873743</v>
+        <v>0.004533473906167633</v>
       </c>
       <c r="E47" t="n">
-        <v>33</v>
+        <v>8.6</v>
       </c>
       <c r="F47" t="n">
-        <v>215.4</v>
+        <v>55.4</v>
       </c>
       <c r="G47" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H47" t="s">
         <v>11</v>
       </c>
       <c r="I47" t="n">
-        <v>0.1187514263010913</v>
+        <v>0.02920400632577754</v>
       </c>
       <c r="J47" t="n">
-        <v>6.2</v>
+        <v>5.6</v>
       </c>
       <c r="K47" t="n">
-        <v>0.003086678567510356</v>
+        <v>0.002952029520295203</v>
       </c>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="1" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>3.47305785123967</v>
+        <v>7.51158683240029</v>
       </c>
       <c r="C48" t="n">
-        <v>6303.6</v>
+        <v>13872.6</v>
       </c>
       <c r="D48" t="n">
-        <v>0.01641873278236915</v>
+        <v>0.05479912609262635</v>
       </c>
       <c r="E48" t="n">
-        <v>29.8</v>
+        <v>100.2</v>
       </c>
       <c r="F48" t="n">
-        <v>48.2</v>
+        <v>247.2</v>
       </c>
       <c r="G48" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H48" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I48" t="n">
-        <v>0.0265564738292011</v>
+        <v>0.1365267651592364</v>
       </c>
       <c r="J48" t="n">
-        <v>3.2</v>
+        <v>13.6</v>
       </c>
       <c r="K48" t="n">
-        <v>0.001763085399449036</v>
+        <v>0.007220297237391181</v>
       </c>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="1" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B49" t="n">
-        <v>3.753610964681075</v>
+        <v>4.572666963511966</v>
       </c>
       <c r="C49" t="n">
-        <v>7120.6</v>
+        <v>6508.2</v>
       </c>
       <c r="D49" t="n">
-        <v>0.004533473906167633</v>
+        <v>0.06072079108439347</v>
       </c>
       <c r="E49" t="n">
-        <v>8.6</v>
+        <v>80.2</v>
       </c>
       <c r="F49" t="n">
-        <v>55.4</v>
+        <v>234.6</v>
       </c>
       <c r="G49" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="H49" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I49" t="n">
-        <v>0.02920400632577754</v>
+        <v>0.1959332610452971</v>
       </c>
       <c r="J49" t="n">
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
       <c r="K49" t="n">
-        <v>0.002952029520295203</v>
+        <v>0.004025397629974161</v>
       </c>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="1" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B50" t="n">
-        <v>7.51158683240029</v>
+        <v>0.4861538461538461</v>
       </c>
       <c r="C50" t="n">
-        <v>13872.6</v>
+        <v>94.8</v>
       </c>
       <c r="D50" t="n">
-        <v>0.05479912609262635</v>
+        <v>0.01128205128205128</v>
       </c>
       <c r="E50" t="n">
-        <v>100.2</v>
+        <v>2.2</v>
       </c>
       <c r="F50" t="n">
-        <v>247.2</v>
+        <v>28</v>
       </c>
       <c r="G50" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H50" t="s">
         <v>18</v>
       </c>
       <c r="I50" t="n">
-        <v>0.1365267651592364</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="J50" t="n">
-        <v>13.6</v>
+        <v>0</v>
       </c>
       <c r="K50" t="n">
-        <v>0.007220297237391181</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="1" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B51" t="n">
-        <v>4.572666963511966</v>
+        <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>6508.2</v>
+        <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>0.06072079108439347</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>80.2</v>
+        <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>234.6</v>
-      </c>
-      <c r="G51" t="s">
-        <v>38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G51" t="s"/>
       <c r="H51" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I51" t="n">
-        <v>0.1959332610452971</v>
+        <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>5.8</v>
+        <v>0</v>
       </c>
       <c r="K51" t="n">
-        <v>0.004025397629974161</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="1" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B52" t="n">
-        <v>0.4861538461538461</v>
+        <v>2.719359230470012</v>
       </c>
       <c r="C52" t="n">
-        <v>94.8</v>
+        <v>3811.5</v>
       </c>
       <c r="D52" t="n">
-        <v>0.01128205128205128</v>
+        <v>0.01770923299731227</v>
       </c>
       <c r="E52" t="n">
-        <v>2.2</v>
+        <v>28.5</v>
       </c>
       <c r="F52" t="n">
-        <v>28</v>
+        <v>279.5</v>
       </c>
       <c r="G52" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="H52" t="s">
+        <v>11</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.1933071592924438</v>
+      </c>
+      <c r="J52" t="n">
         <v>18</v>
       </c>
-      <c r="I52" t="n">
-        <v>0.1435897435897436</v>
-      </c>
-      <c r="J52" t="n">
-        <v>0</v>
-      </c>
       <c r="K52" t="n">
-        <v>0</v>
+        <v>0.01137944447740923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some error catching mechanisms
</commit_message>
<xml_diff>
--- a/lol.xlsx
+++ b/lol.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>Aggression Point</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Poppy Gods</t>
+  </si>
+  <si>
+    <t>Mr Kayn</t>
   </si>
 </sst>
 </file>
@@ -483,7 +486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2063,7 +2066,7 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" t="n">
         <v>2.686192441575164</v>
@@ -2098,7 +2101,7 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="1" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B47" t="n">
         <v>3.753610964681075</v>
@@ -2133,7 +2136,7 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="1" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B48" t="n">
         <v>7.51158683240029</v>
@@ -2168,7 +2171,7 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="1" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B49" t="n">
         <v>4.572666963511966</v>
@@ -2203,7 +2206,7 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="1" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B50" t="n">
         <v>0.4861538461538461</v>
@@ -2238,7 +2241,7 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="1" t="n">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B51" t="n">
         <v>0</v>
@@ -2271,7 +2274,7 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="1" t="n">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B52" t="n">
         <v>2.719359230470012</v>
@@ -2302,6 +2305,249 @@
       </c>
       <c r="K52" t="n">
         <v>0.01137944447740923</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1.775319622012229</v>
+      </c>
+      <c r="C53" t="n">
+        <v>3193.8</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.01634241245136187</v>
+      </c>
+      <c r="E53" t="n">
+        <v>29.4</v>
+      </c>
+      <c r="F53" t="n">
+        <v>41</v>
+      </c>
+      <c r="G53" t="s">
+        <v>12</v>
+      </c>
+      <c r="H53" t="s">
+        <v>11</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.02279043913285158</v>
+      </c>
+      <c r="J53" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.002445803224013341</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="n">
+        <v>7.410958116892823</v>
+      </c>
+      <c r="C54" t="n">
+        <v>13175.2</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.05164043510720542</v>
+      </c>
+      <c r="E54" t="n">
+        <v>91.2</v>
+      </c>
+      <c r="F54" t="n">
+        <v>278.8</v>
+      </c>
+      <c r="G54" t="s">
+        <v>13</v>
+      </c>
+      <c r="H54" t="s">
+        <v>11</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.1567269453783251</v>
+      </c>
+      <c r="J54" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.004627791059971394</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="n">
+        <v>6.474714026753915</v>
+      </c>
+      <c r="C55" t="n">
+        <v>8602</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.04634044514716931</v>
+      </c>
+      <c r="E55" t="n">
+        <v>61.2</v>
+      </c>
+      <c r="F55" t="n">
+        <v>328.6</v>
+      </c>
+      <c r="G55" t="s">
+        <v>14</v>
+      </c>
+      <c r="H55" t="s">
+        <v>11</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.2473481266503256</v>
+      </c>
+      <c r="J55" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.007220967752454279</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.901710291787398</v>
+      </c>
+      <c r="C56" t="n">
+        <v>4185.8</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.01349240180076153</v>
+      </c>
+      <c r="E56" t="n">
+        <v>29.6</v>
+      </c>
+      <c r="F56" t="n">
+        <v>204.4</v>
+      </c>
+      <c r="G56" t="s">
+        <v>15</v>
+      </c>
+      <c r="H56" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.09128055152368671</v>
+      </c>
+      <c r="J56" t="n">
+        <v>18.6</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.008167217339014521</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B57" t="n">
+        <v>2.791646791513082</v>
+      </c>
+      <c r="C57" t="n">
+        <v>3890.6</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.01949175076877424</v>
+      </c>
+      <c r="E57" t="n">
+        <v>28.2</v>
+      </c>
+      <c r="F57" t="n">
+        <v>221.4</v>
+      </c>
+      <c r="G57" t="s">
+        <v>40</v>
+      </c>
+      <c r="H57" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.1749684198889241</v>
+      </c>
+      <c r="J57" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.002463335941977546</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="s"/>
+      <c r="H58" t="s">
+        <v>11</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1.775319622012229</v>
+      </c>
+      <c r="C59" t="n">
+        <v>3193.8</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.01634241245136187</v>
+      </c>
+      <c r="E59" t="n">
+        <v>29.4</v>
+      </c>
+      <c r="F59" t="n">
+        <v>41</v>
+      </c>
+      <c r="G59" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" t="s">
+        <v>11</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.02279043913285158</v>
+      </c>
+      <c r="J59" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.002445803224013341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>